<commit_message>
Updated Measure Units also
</commit_message>
<xml_diff>
--- a/Table Structure.xlsx
+++ b/Table Structure.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NODE\Payment-Records\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NODE\Financial-Ledger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D90CC00-C09B-45CD-818F-034C10BAC984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D877CA9A-B352-43F5-BA6B-E3651E06072F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{BC1AD6E1-B5BF-432E-BF54-B361662FA112}"/>
   </bookViews>
@@ -201,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +247,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -274,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -282,7 +289,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13361C8F-36D5-4D61-B81F-3F71F3981006}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H21" sqref="B21:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -625,7 +633,7 @@
         <v>26</v>
       </c>
       <c r="I1" s="5"/>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -641,10 +649,10 @@
       <c r="I2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -660,10 +668,10 @@
       <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -676,10 +684,10 @@
       <c r="I4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -695,10 +703,10 @@
       <c r="I5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -714,10 +722,10 @@
       <c r="I6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -727,10 +735,10 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="P7" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -741,10 +749,10 @@
       <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P8" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -752,10 +760,10 @@
       <c r="F9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -769,10 +777,10 @@
       <c r="F10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -780,6 +788,7 @@
       <c r="F11" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="P11" s="7"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
@@ -796,100 +805,121 @@
       </c>
       <c r="C13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="7" t="s">
         <v>46</v>
       </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="C14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="L14" s="2" t="s">
+      <c r="K14" s="7"/>
+      <c r="L14" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="K15" s="7"/>
+      <c r="L15" s="7" t="s">
         <v>47</v>
       </c>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="K16" s="7"/>
+      <c r="L16" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
-      <c r="L17" s="2" t="s">
+      <c r="K17" s="7"/>
+      <c r="L17" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" s="7"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="6"/>
-      <c r="L18" s="2" t="s">
+      <c r="K18" s="7"/>
+      <c r="L18" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" s="7"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K20" s="2">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C22" s="2" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="7">
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8">
         <v>0.05</v>
       </c>
-      <c r="K22" s="2">
-        <f>(5/100)*2000</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C23" s="2" t="s">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="7">
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C24" s="2" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="7">
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="8">
         <v>0</v>
       </c>
     </row>

</xml_diff>